<commit_message>
major changes, analytics, reusable questions
</commit_message>
<xml_diff>
--- a/public/template/ess.xlsx
+++ b/public/template/ess.xlsx
@@ -37,49 +37,49 @@
     <t>POINTS</t>
   </si>
   <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>q5</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>q9</t>
-  </si>
-  <si>
-    <t>q10</t>
-  </si>
-  <si>
-    <t>q11</t>
-  </si>
-  <si>
-    <t>q12</t>
-  </si>
-  <si>
-    <t>q13</t>
-  </si>
-  <si>
-    <t>q14</t>
-  </si>
-  <si>
-    <t>q15</t>
-  </si>
-  <si>
-    <t>q1 saddf sdaf sdaflksdjadflsd af jsdafsda jf lsdaflsd flsdajd flsdjal fkjsdal fjsalfjsdlfjsdlfsdka fsdaf</t>
-  </si>
-  <si>
-    <t>asd fsd fsdadf sda fsda fsdaf sadf sdaf sdaf sdaf sda fsda fsdaf sdaf sdafsd fsd</t>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>Question 4</t>
+  </si>
+  <si>
+    <t>Question 5</t>
+  </si>
+  <si>
+    <t>Question 6</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Question 8</t>
+  </si>
+  <si>
+    <t>Question 9</t>
+  </si>
+  <si>
+    <t>Question 10</t>
+  </si>
+  <si>
+    <t>Question 11</t>
+  </si>
+  <si>
+    <t>Question 12</t>
+  </si>
+  <si>
+    <t>Question 13</t>
+  </si>
+  <si>
+    <t>Question 14</t>
+  </si>
+  <si>
+    <t>Question 15</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +514,9 @@
     <col min="1" max="1" width="9.1796875" style="4"/>
     <col min="2" max="2" width="39.26953125" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.81640625" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="5" width="9.1796875" style="4"/>
+    <col min="6" max="6" width="59.08984375" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -542,147 +544,147 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" s="5">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -690,10 +692,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -701,10 +703,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -722,7 +724,7 @@
       <c r="D20" s="10"/>
     </row>
   </sheetData>
-  <sheetProtection password="D692" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="CA9C" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0"/>
   <mergeCells count="2">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A19:D20"/>

</xml_diff>